<commit_message>
working version of eroski with Retrievers iterator class
</commit_message>
<xml_diff>
--- a/precios.xlsx
+++ b/precios.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-11-15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2022-11-19" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
       <c r="D8" t="n">
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="9">
@@ -640,16 +640,8 @@
           <t>ANCHOA FILETE ACEITE OLIVA</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -709,10 +701,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.89</v>
+        <v>3.05</v>
       </c>
       <c r="D17" t="n">
-        <v>2.89</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="18">
@@ -756,16 +748,8 @@
           <t xml:space="preserve">BONITO </t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -953,10 +937,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15.85</v>
+        <v>13.45</v>
       </c>
       <c r="D32" t="n">
-        <v>15.85</v>
+        <v>13.45</v>
       </c>
     </row>
     <row r="33">
@@ -1081,10 +1065,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.75</v>
+        <v>1.99</v>
       </c>
       <c r="D40" t="n">
-        <v>1.75</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="41">
@@ -1224,16 +1208,8 @@
           <t>FAIRY</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1437,10 +1413,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.13</v>
+        <v>1.99</v>
       </c>
       <c r="D62" t="n">
-        <v>2.13</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="63">
@@ -1485,10 +1461,10 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>5.99</v>
+        <v>6.99</v>
       </c>
       <c r="D65" t="n">
-        <v>5.99</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="66">
@@ -1533,10 +1509,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.96</v>
+        <v>1.09</v>
       </c>
       <c r="D68" t="n">
-        <v>0.96</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="69">
@@ -1548,15 +1524,11 @@
           <t>LECHE SEMIDESNATADA</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="C69" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.09</v>
       </c>
     </row>
     <row r="70">
@@ -1569,10 +1541,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.05</v>
+        <v>1.19</v>
       </c>
       <c r="D70" t="n">
-        <v>1.05</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="71">
@@ -1649,10 +1621,10 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2.95</v>
+        <v>3.99</v>
       </c>
       <c r="D75" t="n">
-        <v>2.95</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="76">
@@ -1840,16 +1812,8 @@
           <t xml:space="preserve">MELOCOTON </t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1893,10 +1857,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>14.85</v>
+        <v>16.43</v>
       </c>
       <c r="D90" t="n">
-        <v>14.85</v>
+        <v>16.43</v>
       </c>
     </row>
     <row r="91">
@@ -1925,10 +1889,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1.99</v>
+        <v>1.69</v>
       </c>
       <c r="D92" t="n">
-        <v>1.99</v>
+        <v>1.69</v>
       </c>
     </row>
     <row r="93">
@@ -1940,15 +1904,11 @@
           <t>NATA COCINA</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="C93" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1.75</v>
       </c>
     </row>
     <row r="94">
@@ -1961,10 +1921,10 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>3.59</v>
+        <v>3.99</v>
       </c>
       <c r="D94" t="n">
-        <v>3.59</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="95">
@@ -2056,12 +2016,8 @@
           <t>PATATA ENTERA CONSERVA</t>
         </is>
       </c>
-      <c r="C100" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="D100" t="n">
-        <v>1.35</v>
-      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -2185,10 +2141,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="D108" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
@@ -2201,10 +2157,10 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3.58</v>
+        <v>3.98</v>
       </c>
       <c r="D109" t="n">
-        <v>3.58</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="110">
@@ -2408,15 +2364,11 @@
           <t xml:space="preserve">SALSA BECHAMEL </t>
         </is>
       </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+      <c r="C122" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="D122" t="n">
+        <v>4.27</v>
       </c>
     </row>
     <row r="123">
@@ -2493,10 +2445,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1.15</v>
+        <v>1.28</v>
       </c>
       <c r="D127" t="n">
-        <v>1.15</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="128">
@@ -2509,10 +2461,10 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1.46</v>
+        <v>1.7</v>
       </c>
       <c r="D128" t="n">
-        <v>1.46</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="129">

</xml_diff>